<commit_message>
cleaned folders and updated batchPhoto.py
</commit_message>
<xml_diff>
--- a/excel_sheets/attendance.xlsx
+++ b/excel_sheets/attendance.xlsx
@@ -13,6 +13,7 @@
     <sheet name="2021-09-02" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="2021-09-06" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="2021-09-10" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2021-09-18" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1707,4 +1708,111 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Face_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Heart-rate</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Body_temp</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Ambient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dishant</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Team Lead</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>17:10:59</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>98.83116074550881</v>
+      </c>
+      <c r="G2" t="n">
+        <v>78</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>